<commit_message>
finishd all experiments with enriched and enriched with kw
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts_enriched.xlsx
+++ b/models/evaluations/evaluation_prompts_enriched.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835708A0-79B6-214E-A94E-8CD1F2D074E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBC7902-24E3-C142-868D-3A993A488E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="108">
   <si>
     <t>prompt description</t>
   </si>
@@ -387,18 +387,6 @@
     <t>P11_5</t>
   </si>
   <si>
-    <t>CoT&amp;CC: based upon P11 (CoT placement with best results) but with shortened annotation guidelines</t>
-  </si>
-  <si>
-    <t>CoT&amp;CC: shortened annotation guidelines, only table &amp;Let's think step by step (CoT)</t>
-  </si>
-  <si>
-    <t>CoT&amp;CC: shortened annotation guidelines, only table &amp;Let's think step by step (CoT) put in different place than P11</t>
-  </si>
-  <si>
-    <t>CoT&amp;CC: shortened annotation guidelines, only table &amp;Let's think step by step (CoT) put in different place than P11 and P11_1</t>
-  </si>
-  <si>
     <t>P12</t>
   </si>
   <si>
@@ -427,6 +415,24 @@
   </si>
   <si>
     <t>Binary</t>
+  </si>
+  <si>
+    <t>CC: shortened annotation guidelines, only table; added separate mention of labels; reduced mentions of  1) what classification should apply to and 2) format and changed where those infos occur</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: Let's think step by step &amp; shortened annotation guidelines, only table</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: Let's think step by step (CoT) put in different place than P11 &amp; shortened annotation guidelines, only table</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: Let's think step by step (CoT) put in different place than P11 and P11_1&amp; shortened annotation guidelines, only table</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: based on P11 (CoT placement with best results) but with shortened annotation guidelines</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: based on P11 (CoT placement with best results) but with original annotation guidelines</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,6 +542,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -577,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -611,6 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
   <dimension ref="B2:AU62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -979,24 +992,24 @@
   <sheetData>
     <row r="2" spans="2:47" x14ac:dyDescent="0.2">
       <c r="E2" s="23" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="K2" s="23" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
       <c r="Q2" s="18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="R2" s="18"/>
       <c r="S2" s="18"/>
       <c r="T2" s="17"/>
       <c r="U2" s="6"/>
       <c r="W2" s="18" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="X2" s="18"/>
       <c r="Y2" s="18"/>
@@ -1156,6 +1169,15 @@
       <c r="C5" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="E5">
+        <v>0.440581</v>
+      </c>
+      <c r="F5">
+        <v>0.279026</v>
+      </c>
+      <c r="G5">
+        <v>0.20269999999999999</v>
+      </c>
       <c r="I5" s="8" t="s">
         <v>6</v>
       </c>
@@ -1202,16 +1224,16 @@
         <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="E6" s="25"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="I6" s="9" t="s">
         <v>20</v>
       </c>
       <c r="J6" s="22"/>
-      <c r="K6" s="12"/>
+      <c r="K6" s="25"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
       <c r="O6" s="9" t="s">
@@ -1235,7 +1257,7 @@
         <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -1264,10 +1286,19 @@
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="E8">
+        <v>0.57214100000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.45318399999999998</v>
+      </c>
+      <c r="G8">
+        <v>0.43035400000000001</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>8</v>
@@ -1313,7 +1344,16 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="E9">
+        <v>0.54481500000000005</v>
+      </c>
+      <c r="F9">
+        <v>0.45131100000000002</v>
+      </c>
+      <c r="G9">
+        <v>0.42663400000000001</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>9</v>
@@ -1359,7 +1399,16 @@
         <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="E10">
+        <v>0.55305099999999996</v>
+      </c>
+      <c r="F10">
+        <v>0.43258400000000002</v>
+      </c>
+      <c r="G10">
+        <v>0.39818700000000001</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>10</v>
@@ -1405,7 +1454,16 @@
         <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="E11">
+        <v>0.55785499999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.44756600000000002</v>
+      </c>
+      <c r="G11">
+        <v>0.42685800000000002</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>21</v>
@@ -1447,7 +1505,7 @@
         <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -1479,7 +1537,16 @@
         <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="E13">
+        <v>0.55179900000000004</v>
+      </c>
+      <c r="F13">
+        <v>0.43445699999999998</v>
+      </c>
+      <c r="G13">
+        <v>0.41641499999999998</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>12</v>
@@ -1535,7 +1602,16 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="E14">
+        <v>0.49582300000000001</v>
+      </c>
+      <c r="F14">
+        <v>0.413858</v>
+      </c>
+      <c r="G14">
+        <v>0.39160699999999998</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>13</v>
@@ -1575,6 +1651,15 @@
       <c r="C15" s="11" t="s">
         <v>42</v>
       </c>
+      <c r="E15">
+        <v>0.60822500000000002</v>
+      </c>
+      <c r="F15">
+        <v>0.51123600000000002</v>
+      </c>
+      <c r="G15">
+        <v>0.498251</v>
+      </c>
       <c r="I15" s="8" t="s">
         <v>14</v>
       </c>
@@ -1623,6 +1708,15 @@
       </c>
       <c r="C16" s="11" t="s">
         <v>46</v>
+      </c>
+      <c r="E16">
+        <v>0.59108099999999997</v>
+      </c>
+      <c r="F16">
+        <v>0.54119899999999999</v>
+      </c>
+      <c r="G16">
+        <v>0.53234800000000004</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>15</v>
@@ -1676,6 +1770,15 @@
       <c r="C17" s="11" t="s">
         <v>58</v>
       </c>
+      <c r="E17">
+        <v>0.45730599999999999</v>
+      </c>
+      <c r="F17">
+        <v>0.30524299999999999</v>
+      </c>
+      <c r="G17">
+        <v>0.22872300000000001</v>
+      </c>
       <c r="I17" s="8" t="s">
         <v>16</v>
       </c>
@@ -1725,7 +1828,7 @@
         <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -1757,7 +1860,16 @@
         <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="E19">
+        <v>0.53071400000000002</v>
+      </c>
+      <c r="F19">
+        <v>0.41011199999999998</v>
+      </c>
+      <c r="G19">
+        <v>0.37525199999999997</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>18</v>
@@ -1792,16 +1904,25 @@
     </row>
     <row r="20" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C20" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" t="s">
         <v>98</v>
       </c>
-      <c r="D20" t="s">
-        <v>102</v>
+      <c r="E20">
+        <v>0.51036099999999995</v>
+      </c>
+      <c r="F20">
+        <v>0.40636699999999998</v>
+      </c>
+      <c r="G20">
+        <v>0.37501000000000001</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J20" s="22"/>
       <c r="K20">
@@ -1814,7 +1935,7 @@
         <v>0.39521200000000001</v>
       </c>
       <c r="O20" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="Q20">
         <v>0.52865600000000001</v>
@@ -1838,6 +1959,15 @@
       <c r="C21" s="11" t="s">
         <v>33</v>
       </c>
+      <c r="E21">
+        <v>0.47591099999999997</v>
+      </c>
+      <c r="F21">
+        <v>0.353933</v>
+      </c>
+      <c r="G21">
+        <v>0.29121799999999998</v>
+      </c>
       <c r="I21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1874,7 +2004,16 @@
         <v>25</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>93</v>
+        <v>103</v>
+      </c>
+      <c r="E22">
+        <v>0.57200399999999996</v>
+      </c>
+      <c r="F22">
+        <v>0.44194800000000001</v>
+      </c>
+      <c r="G22">
+        <v>0.41675600000000002</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>25</v>
@@ -1912,10 +2051,19 @@
         <v>26</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="E23">
+        <v>0.57674099999999995</v>
+      </c>
+      <c r="F23">
+        <v>0.45131100000000002</v>
+      </c>
+      <c r="G23">
+        <v>0.42775800000000003</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>26</v>
@@ -1953,10 +2101,19 @@
         <v>27</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D24" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="E24">
+        <v>0.57912399999999997</v>
+      </c>
+      <c r="F24">
+        <v>0.46254699999999999</v>
+      </c>
+      <c r="G24">
+        <v>0.44266699999999998</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>27</v>
@@ -1997,12 +2154,30 @@
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="E25">
+        <v>0.63638499999999998</v>
+      </c>
+      <c r="F25">
+        <v>0.503745</v>
+      </c>
+      <c r="G25">
+        <v>0.48842400000000002</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>28</v>
       </c>
       <c r="J25" s="22"/>
+      <c r="K25">
+        <v>0.61878200000000005</v>
+      </c>
+      <c r="L25">
+        <v>0.50936300000000001</v>
+      </c>
+      <c r="M25">
+        <v>0.48682399999999998</v>
+      </c>
       <c r="O25" s="8" t="s">
         <v>28</v>
       </c>
@@ -2038,15 +2213,33 @@
         <v>29</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="E26">
+        <v>0.60144699999999995</v>
+      </c>
+      <c r="F26">
+        <v>0.52808999999999995</v>
+      </c>
+      <c r="G26">
+        <v>0.518258</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J26" s="22"/>
+      <c r="K26">
+        <v>0.58768200000000004</v>
+      </c>
+      <c r="L26">
+        <v>0.51872700000000005</v>
+      </c>
+      <c r="M26">
+        <v>0.508934</v>
+      </c>
       <c r="O26" s="8" t="s">
         <v>29</v>
       </c>
@@ -2081,15 +2274,33 @@
         <v>91</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="E27">
+        <v>0.55141600000000002</v>
+      </c>
+      <c r="F27">
+        <v>0.42509400000000003</v>
+      </c>
+      <c r="G27">
+        <v>0.40416999999999997</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>91</v>
       </c>
       <c r="J27" s="22"/>
+      <c r="K27">
+        <v>0.54432199999999997</v>
+      </c>
+      <c r="L27">
+        <v>0.417603</v>
+      </c>
+      <c r="M27">
+        <v>0.39237300000000003</v>
+      </c>
       <c r="O27" s="8" t="s">
         <v>91</v>
       </c>
@@ -2110,17 +2321,35 @@
     </row>
     <row r="28" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>99</v>
+        <v>95</v>
+      </c>
+      <c r="E28">
+        <v>0.52750699999999995</v>
+      </c>
+      <c r="F28">
+        <v>0.40262199999999998</v>
+      </c>
+      <c r="G28">
+        <v>0.37142799999999998</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J28" s="22"/>
+      <c r="K28">
+        <v>0.51415699999999998</v>
+      </c>
+      <c r="L28">
+        <v>0.39513100000000001</v>
+      </c>
+      <c r="M28">
+        <v>0.36011399999999999</v>
+      </c>
       <c r="O28" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="Q28">
         <v>0.55375399999999997</v>
@@ -2148,15 +2377,15 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B36" s="24" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F36" s="23"/>
       <c r="G36" s="23"/>
       <c r="K36" s="23" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L36" s="23"/>
       <c r="M36" s="23"/>
@@ -2303,7 +2532,7 @@
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C54" s="11"/>
     </row>
@@ -2351,7 +2580,7 @@
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B62" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C62" s="11"/>
     </row>

</xml_diff>

<commit_message>
P1, P4, P5 auf gpt-4 mit enriched_kw laufen lassen
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts_enriched.xlsx
+++ b/models/evaluations/evaluation_prompts_enriched.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBC7902-24E3-C142-868D-3A993A488E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734ED34A-9A29-4A46-A23D-94D063143847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="109">
   <si>
     <t>prompt description</t>
   </si>
@@ -434,12 +434,15 @@
   <si>
     <t>CoT&amp;CC: based on P11 (CoT placement with best results) but with original annotation guidelines</t>
   </si>
+  <si>
+    <t>summary enriched_kw_0.2test_gpt-4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -484,6 +487,12 @@
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -589,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -612,6 +621,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -619,11 +630,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
   <dimension ref="B2:AU62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:G28"/>
+    <sheetView tabSelected="1" topLeftCell="M11" zoomScale="136" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -991,43 +999,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:47" x14ac:dyDescent="0.2">
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="K2" s="23" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="K2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="Q2" s="18" t="s">
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="Q2" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
       <c r="T2" s="17"/>
       <c r="U2" s="6"/>
-      <c r="W2" s="18" t="s">
+      <c r="W2" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="17"/>
+      <c r="AC2" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="17"/>
-      <c r="AC2" s="18"/>
-      <c r="AD2" s="18"/>
-      <c r="AE2" s="18"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
       <c r="AF2" s="6"/>
       <c r="AG2" s="6"/>
-      <c r="AI2" s="18"/>
-      <c r="AJ2" s="18"/>
-      <c r="AK2" s="18"/>
-      <c r="AN2" s="18"/>
-      <c r="AO2" s="18"/>
-      <c r="AP2" s="18"/>
-      <c r="AS2" s="18"/>
-      <c r="AT2" s="18"/>
-      <c r="AU2" s="18"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AN2" s="20"/>
+      <c r="AO2" s="20"/>
+      <c r="AP2" s="20"/>
+      <c r="AS2" s="20"/>
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="20"/>
     </row>
     <row r="3" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
@@ -1070,7 +1080,9 @@
         <v>4</v>
       </c>
       <c r="T3" s="1"/>
-      <c r="U3" s="7"/>
+      <c r="U3" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="W3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1080,12 +1092,20 @@
       <c r="Y3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="7"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
+      <c r="AA3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AF3" s="1"/>
-      <c r="AG3" s="7"/>
+      <c r="AG3" s="23"/>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
@@ -1117,14 +1137,13 @@
       <c r="I4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="22"/>
       <c r="K4">
         <v>0.46124900000000002</v>
       </c>
       <c r="L4">
         <v>0.34082400000000002</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="14">
         <v>0.271316</v>
       </c>
       <c r="O4" s="8" t="s">
@@ -1139,23 +1158,33 @@
       <c r="S4">
         <v>0.210198</v>
       </c>
-      <c r="U4" s="8"/>
+      <c r="U4" s="8" t="s">
+        <v>5</v>
+      </c>
       <c r="V4" s="16"/>
       <c r="W4">
+        <v>0.54401100000000002</v>
+      </c>
+      <c r="X4">
+        <v>0.47191</v>
+      </c>
+      <c r="Y4">
+        <v>0.42808000000000002</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC4">
         <v>0.58704400000000001</v>
       </c>
-      <c r="X4">
+      <c r="AD4">
         <v>0.41336600000000001</v>
       </c>
-      <c r="Y4">
+      <c r="AE4">
         <v>0.39852399999999999</v>
       </c>
-      <c r="AA4" s="8"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
-      <c r="AG4" s="8"/>
+      <c r="AG4" s="23"/>
       <c r="AI4" s="2"/>
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
@@ -1181,7 +1210,6 @@
       <c r="I5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="22"/>
       <c r="K5">
         <v>0.42036200000000001</v>
       </c>
@@ -1203,13 +1231,14 @@
       <c r="S5">
         <v>0.17084299999999999</v>
       </c>
-      <c r="U5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
+      <c r="U5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA5" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="AF5" s="2"/>
-      <c r="AG5" s="8"/>
+      <c r="AG5" s="23"/>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
@@ -1226,14 +1255,13 @@
       <c r="D6" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="I6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="25"/>
+      <c r="K6" s="19"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
       <c r="O6" s="9" t="s">
@@ -1243,9 +1271,13 @@
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
       <c r="T6" s="2"/>
-      <c r="U6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AG6" s="9"/>
+      <c r="U6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG6" s="24"/>
       <c r="AM6" s="9"/>
       <c r="AR6" s="9"/>
     </row>
@@ -1265,7 +1297,6 @@
       <c r="I7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="22"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
@@ -1275,9 +1306,13 @@
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
-      <c r="U7" s="9"/>
-      <c r="AA7" s="9"/>
-      <c r="AG7" s="9"/>
+      <c r="U7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG7" s="24"/>
       <c r="AM7" s="9"/>
       <c r="AR7" s="9"/>
     </row>
@@ -1297,13 +1332,12 @@
       <c r="F8">
         <v>0.45318399999999998</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="14">
         <v>0.43035400000000001</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="22"/>
       <c r="K8">
         <v>0.55821900000000002</v>
       </c>
@@ -1326,13 +1360,14 @@
         <v>0.29668600000000001</v>
       </c>
       <c r="T8" s="2"/>
-      <c r="U8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
+      <c r="U8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA8" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="AF8" s="2"/>
-      <c r="AG8" s="8"/>
+      <c r="AG8" s="23"/>
       <c r="AM8" s="8"/>
       <c r="AR8" s="8"/>
     </row>
@@ -1352,13 +1387,12 @@
       <c r="F9">
         <v>0.45131100000000002</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="14">
         <v>0.42663400000000001</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="22"/>
       <c r="K9">
         <v>0.53802099999999997</v>
       </c>
@@ -1381,13 +1415,14 @@
         <v>0.29295399999999999</v>
       </c>
       <c r="T9" s="2"/>
-      <c r="U9" s="8"/>
-      <c r="AA9" s="8"/>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
+      <c r="U9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA9" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="AF9" s="2"/>
-      <c r="AG9" s="8"/>
+      <c r="AG9" s="23"/>
       <c r="AM9" s="8"/>
       <c r="AR9" s="8"/>
     </row>
@@ -1413,14 +1448,13 @@
       <c r="I10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="22"/>
       <c r="K10">
         <v>0.53802099999999997</v>
       </c>
       <c r="L10">
         <v>0.44756600000000002</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="14">
         <v>0.41922799999999999</v>
       </c>
       <c r="O10" s="8" t="s">
@@ -1436,13 +1470,14 @@
         <v>0.269202</v>
       </c>
       <c r="T10" s="2"/>
-      <c r="U10" s="8"/>
-      <c r="AA10" s="8"/>
-      <c r="AC10" s="2"/>
-      <c r="AD10" s="2"/>
-      <c r="AE10" s="2"/>
+      <c r="U10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA10" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="AF10" s="2"/>
-      <c r="AG10" s="8"/>
+      <c r="AG10" s="23"/>
       <c r="AM10" s="8"/>
       <c r="AR10" s="8"/>
     </row>
@@ -1468,14 +1503,13 @@
       <c r="I11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="22"/>
       <c r="K11">
         <v>0.58662300000000001</v>
       </c>
       <c r="L11">
         <v>0.45880100000000001</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="14">
         <v>0.44216800000000001</v>
       </c>
       <c r="O11" s="8" t="s">
@@ -1491,9 +1525,13 @@
         <v>0.297539</v>
       </c>
       <c r="T11" s="2"/>
-      <c r="U11" s="8"/>
-      <c r="AA11" s="8"/>
-      <c r="AG11" s="8"/>
+      <c r="U11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG11" s="23"/>
       <c r="AM11" s="8"/>
       <c r="AR11" s="8"/>
     </row>
@@ -1513,7 +1551,6 @@
       <c r="I12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="22"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
@@ -1523,9 +1560,13 @@
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
-      <c r="U12" s="9"/>
-      <c r="AA12" s="9"/>
-      <c r="AG12" s="9"/>
+      <c r="U12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG12" s="24"/>
       <c r="AM12" s="9"/>
       <c r="AR12" s="9"/>
     </row>
@@ -1545,13 +1586,12 @@
       <c r="F13">
         <v>0.43445699999999998</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="14">
         <v>0.41641499999999998</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="22"/>
       <c r="K13">
         <v>0.56189900000000004</v>
       </c>
@@ -1574,23 +1614,33 @@
         <v>0.34911799999999998</v>
       </c>
       <c r="T13" s="2"/>
-      <c r="U13" s="8"/>
+      <c r="U13" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="V13" s="16"/>
       <c r="W13">
+        <v>0.62507699999999999</v>
+      </c>
+      <c r="X13">
+        <v>0.55618000000000001</v>
+      </c>
+      <c r="Y13">
+        <v>0.53358399999999995</v>
+      </c>
+      <c r="AA13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC13">
         <v>0.69281700000000002</v>
       </c>
-      <c r="X13">
+      <c r="AD13">
         <v>0.53712899999999997</v>
       </c>
-      <c r="Y13">
+      <c r="AE13">
         <v>0.556975</v>
       </c>
-      <c r="AA13" s="8"/>
-      <c r="AC13" s="2"/>
-      <c r="AD13" s="2"/>
-      <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
-      <c r="AG13" s="8"/>
+      <c r="AG13" s="23"/>
       <c r="AM13" s="8"/>
       <c r="AR13" s="8"/>
     </row>
@@ -1616,14 +1666,13 @@
       <c r="I14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="22"/>
       <c r="K14">
         <v>0.54681400000000002</v>
       </c>
       <c r="L14">
         <v>0.43071199999999998</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="14">
         <v>0.41199799999999998</v>
       </c>
       <c r="O14" s="8" t="s">
@@ -1638,9 +1687,13 @@
       <c r="S14">
         <v>0.319803</v>
       </c>
-      <c r="U14" s="8"/>
-      <c r="AA14" s="8"/>
-      <c r="AG14" s="8"/>
+      <c r="U14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG14" s="23"/>
       <c r="AM14" s="8"/>
       <c r="AR14" s="8"/>
     </row>
@@ -1657,13 +1710,12 @@
       <c r="F15">
         <v>0.51123600000000002</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="14">
         <v>0.498251</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="22"/>
       <c r="K15">
         <v>0.62534100000000004</v>
       </c>
@@ -1686,19 +1738,32 @@
         <v>0.41343099999999999</v>
       </c>
       <c r="T15" s="2"/>
-      <c r="U15" s="8"/>
+      <c r="U15" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="V15" s="15"/>
       <c r="W15">
+        <v>0.68644300000000003</v>
+      </c>
+      <c r="X15">
+        <v>0.59175999999999995</v>
+      </c>
+      <c r="Y15">
+        <v>0.58773699999999995</v>
+      </c>
+      <c r="AA15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC15">
         <v>0.691137</v>
       </c>
-      <c r="X15">
+      <c r="AD15">
         <v>0.53217800000000004</v>
       </c>
-      <c r="Y15">
+      <c r="AE15">
         <v>0.55549099999999996</v>
       </c>
-      <c r="AA15" s="8"/>
-      <c r="AG15" s="8"/>
+      <c r="AG15" s="23"/>
       <c r="AM15" s="8"/>
       <c r="AR15" s="8"/>
     </row>
@@ -1715,13 +1780,12 @@
       <c r="F16">
         <v>0.54119899999999999</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="14">
         <v>0.53234800000000004</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="22"/>
       <c r="K16">
         <v>0.57320499999999996</v>
       </c>
@@ -1743,20 +1807,24 @@
       <c r="S16">
         <v>0.47761999999999999</v>
       </c>
-      <c r="T16" s="21"/>
-      <c r="U16" s="8"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="V16" s="15"/>
-      <c r="W16" s="14">
+      <c r="AA16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC16" s="14">
         <v>0.70457400000000003</v>
       </c>
-      <c r="X16" s="14">
+      <c r="AD16" s="14">
         <v>0.53712899999999997</v>
       </c>
-      <c r="Y16" s="14">
+      <c r="AE16" s="14">
         <v>0.57348399999999999</v>
       </c>
-      <c r="AA16" s="8"/>
-      <c r="AG16" s="8"/>
+      <c r="AG16" s="23"/>
       <c r="AM16" s="8"/>
       <c r="AR16" s="8"/>
       <c r="AS16" s="2"/>
@@ -1776,13 +1844,12 @@
       <c r="F17">
         <v>0.30524299999999999</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="14">
         <v>0.22872300000000001</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="22"/>
       <c r="K17">
         <v>0.44090699999999999</v>
       </c>
@@ -1804,19 +1871,23 @@
       <c r="S17">
         <v>0.191112</v>
       </c>
-      <c r="U17" s="8"/>
+      <c r="U17" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="V17" s="16"/>
-      <c r="W17">
+      <c r="AA17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC17">
         <v>0.58668799999999999</v>
       </c>
-      <c r="X17">
+      <c r="AD17">
         <v>0.38861400000000001</v>
       </c>
-      <c r="Y17">
+      <c r="AE17">
         <v>0.34958600000000001</v>
       </c>
-      <c r="AA17" s="8"/>
-      <c r="AG17" s="8"/>
+      <c r="AG17" s="23"/>
       <c r="AM17" s="8"/>
       <c r="AR17" s="8"/>
     </row>
@@ -1836,7 +1907,6 @@
       <c r="I18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="22"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
@@ -1846,9 +1916,13 @@
       <c r="Q18" s="12"/>
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
-      <c r="U18" s="9"/>
-      <c r="AA18" s="9"/>
-      <c r="AG18" s="9"/>
+      <c r="U18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG18" s="24"/>
       <c r="AM18" s="9"/>
       <c r="AR18" s="9"/>
     </row>
@@ -1868,13 +1942,12 @@
       <c r="F19">
         <v>0.41011199999999998</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="14">
         <v>0.37525199999999997</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="22"/>
       <c r="K19">
         <v>0.52873999999999999</v>
       </c>
@@ -1896,9 +1969,13 @@
       <c r="S19">
         <v>0.237849</v>
       </c>
-      <c r="U19" s="8"/>
-      <c r="AA19" s="8"/>
-      <c r="AG19" s="8"/>
+      <c r="U19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG19" s="23"/>
       <c r="AM19" s="8"/>
       <c r="AR19" s="8"/>
     </row>
@@ -1924,14 +2001,13 @@
       <c r="I20" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="J20" s="22"/>
       <c r="K20">
         <v>0.547925</v>
       </c>
       <c r="L20">
         <v>0.42322100000000001</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="14">
         <v>0.39521200000000001</v>
       </c>
       <c r="O20" s="8" t="s">
@@ -1946,9 +2022,13 @@
       <c r="S20">
         <v>0.26192700000000002</v>
       </c>
-      <c r="U20" s="8"/>
-      <c r="AA20" s="8"/>
-      <c r="AG20" s="8"/>
+      <c r="U20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG20" s="23"/>
       <c r="AM20" s="8"/>
       <c r="AR20" s="8"/>
     </row>
@@ -1965,13 +2045,12 @@
       <c r="F21">
         <v>0.353933</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="14">
         <v>0.29121799999999998</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="22"/>
       <c r="K21">
         <v>0.46595500000000001</v>
       </c>
@@ -1993,9 +2072,13 @@
       <c r="S21">
         <v>0.25231799999999999</v>
       </c>
-      <c r="U21" s="8"/>
-      <c r="AA21" s="8"/>
-      <c r="AG21" s="8"/>
+      <c r="U21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG21" s="23"/>
       <c r="AM21" s="8"/>
       <c r="AR21" s="8"/>
     </row>
@@ -2018,14 +2101,13 @@
       <c r="I22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="22"/>
       <c r="K22">
         <v>0.541269</v>
       </c>
       <c r="L22">
         <v>0.449438</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="14">
         <v>0.42220000000000002</v>
       </c>
       <c r="O22" s="8" t="s">
@@ -2040,9 +2122,13 @@
       <c r="S22">
         <v>0.30395699999999998</v>
       </c>
-      <c r="U22" s="8"/>
-      <c r="AA22" s="8"/>
-      <c r="AG22" s="8"/>
+      <c r="U22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG22" s="23"/>
       <c r="AM22" s="8"/>
       <c r="AR22" s="8"/>
     </row>
@@ -2068,14 +2154,13 @@
       <c r="I23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="22"/>
       <c r="K23">
         <v>0.57905399999999996</v>
       </c>
       <c r="L23">
         <v>0.46441900000000003</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="14">
         <v>0.44628299999999999</v>
       </c>
       <c r="O23" s="8" t="s">
@@ -2090,9 +2175,13 @@
       <c r="S23">
         <v>0.28628999999999999</v>
       </c>
-      <c r="U23" s="8"/>
-      <c r="AA23" s="8"/>
-      <c r="AG23" s="8"/>
+      <c r="U23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG23" s="23"/>
       <c r="AM23" s="8"/>
       <c r="AR23" s="8"/>
     </row>
@@ -2112,13 +2201,12 @@
       <c r="F24">
         <v>0.46254699999999999</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="14">
         <v>0.44266699999999998</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J24" s="22"/>
       <c r="K24">
         <v>0.58247599999999999</v>
       </c>
@@ -2140,9 +2228,13 @@
       <c r="S24">
         <v>0.27839900000000001</v>
       </c>
-      <c r="U24" s="8"/>
-      <c r="AA24" s="8"/>
-      <c r="AG24" s="8"/>
+      <c r="U24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG24" s="23"/>
       <c r="AM24" s="8"/>
       <c r="AR24" s="8"/>
     </row>
@@ -2162,13 +2254,12 @@
       <c r="F25">
         <v>0.503745</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="14">
         <v>0.48842400000000002</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J25" s="22"/>
       <c r="K25">
         <v>0.61878200000000005</v>
       </c>
@@ -2191,20 +2282,24 @@
         <v>0.41634399999999999</v>
       </c>
       <c r="T25" s="2"/>
-      <c r="U25" s="8"/>
+      <c r="U25" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="V25" s="16"/>
-      <c r="W25">
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC25">
         <v>0.69020999999999999</v>
       </c>
-      <c r="X25">
+      <c r="AD25">
         <v>0.54455399999999998</v>
       </c>
-      <c r="Y25">
+      <c r="AE25">
         <v>0.560608</v>
       </c>
-      <c r="Z25" s="5"/>
-      <c r="AA25" s="8"/>
-      <c r="AG25" s="8"/>
+      <c r="AG25" s="23"/>
       <c r="AM25" s="8"/>
       <c r="AR25" s="8"/>
     </row>
@@ -2224,13 +2319,12 @@
       <c r="F26">
         <v>0.52808999999999995</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="14">
         <v>0.518258</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J26" s="22"/>
       <c r="K26">
         <v>0.58768200000000004</v>
       </c>
@@ -2253,19 +2347,23 @@
         <v>0.42550700000000002</v>
       </c>
       <c r="T26" s="2"/>
-      <c r="U26" s="8"/>
+      <c r="U26" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="V26" s="16"/>
-      <c r="W26">
+      <c r="AA26" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC26">
         <v>0.69849899999999998</v>
       </c>
-      <c r="X26">
+      <c r="AD26">
         <v>0.54207899999999998</v>
       </c>
-      <c r="Y26">
+      <c r="AE26">
         <v>0.57139099999999998</v>
       </c>
-      <c r="AA26" s="8"/>
-      <c r="AG26" s="8"/>
+      <c r="AG26" s="23"/>
       <c r="AM26" s="8"/>
       <c r="AR26" s="8"/>
     </row>
@@ -2285,13 +2383,12 @@
       <c r="F27">
         <v>0.42509400000000003</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="14">
         <v>0.40416999999999997</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="J27" s="22"/>
       <c r="K27">
         <v>0.54432199999999997</v>
       </c>
@@ -2313,9 +2410,13 @@
       <c r="S27">
         <v>0.34517799999999998</v>
       </c>
-      <c r="U27" s="8"/>
-      <c r="AA27" s="8"/>
-      <c r="AG27" s="8"/>
+      <c r="U27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG27" s="23"/>
       <c r="AM27" s="8"/>
       <c r="AR27" s="8"/>
     </row>
@@ -2332,13 +2433,12 @@
       <c r="F28">
         <v>0.40262199999999998</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="14">
         <v>0.37142799999999998</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="J28" s="22"/>
       <c r="K28">
         <v>0.51415699999999998</v>
       </c>
@@ -2360,12 +2460,19 @@
       <c r="S28">
         <v>0.24971199999999999</v>
       </c>
-      <c r="U28" s="8"/>
-      <c r="AA28" s="8"/>
-      <c r="AG28" s="8"/>
+      <c r="U28" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA28" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG28" s="23"/>
       <c r="AM28" s="8"/>
       <c r="AR28" s="8"/>
     </row>
+    <row r="29" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AG29" s="23"/>
+    </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K33" s="1"/>
     </row>
@@ -2376,19 +2483,19 @@
       <c r="K35" s="1"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="K36" s="23" t="s">
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="K36" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
@@ -2589,9 +2696,9 @@
     <mergeCell ref="AN2:AP2"/>
     <mergeCell ref="AS2:AU2"/>
     <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="AC2:AE2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4514,8 +4621,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4589,20 +4696,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="G1" s="20" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="G1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -5205,20 +5312,20 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="G43" s="20" t="s">
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="G43" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">

</xml_diff>

<commit_message>
redid all gpt-experiments because fuzzy mapping changed a little bit; only 12 prompts on unenriched test-dataset missing
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts_enriched.xlsx
+++ b/models/evaluations/evaluation_prompts_enriched.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734ED34A-9A29-4A46-A23D-94D063143847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BC0AE3-960C-5142-B275-C44400376388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22360" windowHeight="15500" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation_Summary" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="119">
   <si>
     <t>prompt description</t>
   </si>
@@ -399,9 +399,6 @@
     <t>2CoT&amp;CC: P11 &amp; explanation (CoT) based on P9</t>
   </si>
   <si>
-    <t>summary 0.2test gpt-3.5</t>
-  </si>
-  <si>
     <t>summary 0.2test gpt-4</t>
   </si>
   <si>
@@ -436,13 +433,46 @@
   </si>
   <si>
     <t>summary enriched_kw_0.2test_gpt-4</t>
+  </si>
+  <si>
+    <t>P12_1</t>
+  </si>
+  <si>
+    <t>P12_2</t>
+  </si>
+  <si>
+    <t>2CoT&amp;CC: P11_3 (second-best performance of all P11s) &amp; explanation (CoT) based on P9</t>
+  </si>
+  <si>
+    <t>2CoT&amp;CC: P11_4(best performance of all P11s) &amp; explanation (CoT) based on P9</t>
+  </si>
+  <si>
+    <t>summary enriched_0.2test_gpt-3.5 - not re-run with new Fuzzy-Match except 12_1 and 12_2</t>
+  </si>
+  <si>
+    <t>kw</t>
+  </si>
+  <si>
+    <t>without kw</t>
+  </si>
+  <si>
+    <t>kw, gpt-4</t>
+  </si>
+  <si>
+    <t>unenriched</t>
+  </si>
+  <si>
+    <t>summary 0.2test gpt-3.5 without (fuzzy match, unenriched)</t>
+  </si>
+  <si>
+    <t>summary 0.2test gpt-3.5 (with Fuzzy Match)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -495,8 +525,15 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,8 +594,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCC8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -594,11 +637,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -623,6 +677,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,8 +685,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,6 +699,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCC8"/>
       <color rgb="FFFF9699"/>
     </mruColors>
   </colors>
@@ -971,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
-  <dimension ref="B2:AU62"/>
+  <dimension ref="A1:AU62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M11" zoomScale="136" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28:T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -998,46 +1058,60 @@
     <col min="43" max="43" width="2.83203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:47" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R1" t="s">
+        <v>116</v>
+      </c>
+      <c r="X1" t="s">
+        <v>115</v>
+      </c>
+    </row>
     <row r="2" spans="2:47" x14ac:dyDescent="0.2">
       <c r="E2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="Q2" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
+      <c r="Q2" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
       <c r="T2" s="17"/>
       <c r="U2" s="6"/>
-      <c r="W2" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
+      <c r="W2" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
       <c r="Z2" s="17"/>
-      <c r="AC2" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
+      <c r="AC2" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD2" s="21"/>
+      <c r="AE2" s="21"/>
       <c r="AF2" s="6"/>
       <c r="AG2" s="6"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
-      <c r="AS2" s="20"/>
-      <c r="AT2" s="20"/>
-      <c r="AU2" s="20"/>
+      <c r="AI2" s="21"/>
+      <c r="AJ2" s="21"/>
+      <c r="AK2" s="21"/>
+      <c r="AN2" s="21"/>
+      <c r="AO2" s="21"/>
+      <c r="AP2" s="21"/>
+      <c r="AS2" s="21"/>
+      <c r="AT2" s="21"/>
+      <c r="AU2" s="21"/>
     </row>
     <row r="3" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
@@ -1105,7 +1179,7 @@
         <v>4</v>
       </c>
       <c r="AF3" s="1"/>
-      <c r="AG3" s="23"/>
+      <c r="AG3" s="2"/>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
@@ -1150,13 +1224,13 @@
         <v>5</v>
       </c>
       <c r="Q4">
-        <v>0.469831</v>
+        <v>0.469634</v>
       </c>
       <c r="R4">
         <v>0.25742599999999999</v>
       </c>
       <c r="S4">
-        <v>0.210198</v>
+        <v>0.20993300000000001</v>
       </c>
       <c r="U4" s="8" t="s">
         <v>5</v>
@@ -1184,7 +1258,7 @@
         <v>0.39852399999999999</v>
       </c>
       <c r="AF4" s="2"/>
-      <c r="AG4" s="23"/>
+      <c r="AG4" s="2"/>
       <c r="AI4" s="2"/>
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
@@ -1204,7 +1278,7 @@
       <c r="F5">
         <v>0.279026</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="14">
         <v>0.20269999999999999</v>
       </c>
       <c r="I5" s="8" t="s">
@@ -1223,13 +1297,13 @@
         <v>6</v>
       </c>
       <c r="Q5">
-        <v>0.65417800000000004</v>
+        <v>0.65412899999999996</v>
       </c>
       <c r="R5">
         <v>0.225248</v>
       </c>
       <c r="S5">
-        <v>0.17084299999999999</v>
+        <v>0.170764</v>
       </c>
       <c r="U5" s="8" t="s">
         <v>6</v>
@@ -1238,7 +1312,7 @@
         <v>6</v>
       </c>
       <c r="AF5" s="2"/>
-      <c r="AG5" s="23"/>
+      <c r="AG5" s="2"/>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
@@ -1253,11 +1327,11 @@
         <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
       <c r="I6" s="9" t="s">
         <v>20</v>
       </c>
@@ -1277,7 +1351,7 @@
       <c r="AA6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AG6" s="24"/>
+      <c r="AG6" s="20"/>
       <c r="AM6" s="9"/>
       <c r="AR6" s="9"/>
     </row>
@@ -1289,11 +1363,11 @@
         <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
       <c r="I7" s="9" t="s">
         <v>7</v>
       </c>
@@ -1312,7 +1386,7 @@
       <c r="AA7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AG7" s="24"/>
+      <c r="AG7" s="20"/>
       <c r="AM7" s="9"/>
       <c r="AR7" s="9"/>
     </row>
@@ -1321,10 +1395,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E8">
         <v>0.57214100000000001</v>
@@ -1351,13 +1425,13 @@
         <v>8</v>
       </c>
       <c r="Q8">
-        <v>0.59226599999999996</v>
+        <v>0.59009999999999996</v>
       </c>
       <c r="R8">
-        <v>0.31930700000000001</v>
+        <v>0.36881199999999997</v>
       </c>
       <c r="S8">
-        <v>0.29668600000000001</v>
+        <v>0.35915000000000002</v>
       </c>
       <c r="T8" s="2"/>
       <c r="U8" s="8" t="s">
@@ -1367,7 +1441,7 @@
         <v>8</v>
       </c>
       <c r="AF8" s="2"/>
-      <c r="AG8" s="23"/>
+      <c r="AG8" s="2"/>
       <c r="AM8" s="8"/>
       <c r="AR8" s="8"/>
     </row>
@@ -1379,7 +1453,7 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9">
         <v>0.54481500000000005</v>
@@ -1406,13 +1480,13 @@
         <v>9</v>
       </c>
       <c r="Q9">
-        <v>0.48905399999999999</v>
+        <v>0.59520099999999998</v>
       </c>
       <c r="R9">
-        <v>0.31188100000000002</v>
+        <v>0.37623800000000002</v>
       </c>
       <c r="S9">
-        <v>0.29295399999999999</v>
+        <v>0.372693</v>
       </c>
       <c r="T9" s="2"/>
       <c r="U9" s="8" t="s">
@@ -1422,7 +1496,7 @@
         <v>9</v>
       </c>
       <c r="AF9" s="2"/>
-      <c r="AG9" s="23"/>
+      <c r="AG9" s="2"/>
       <c r="AM9" s="8"/>
       <c r="AR9" s="8"/>
     </row>
@@ -1434,16 +1508,16 @@
         <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10">
-        <v>0.55305099999999996</v>
-      </c>
-      <c r="F10">
-        <v>0.43258400000000002</v>
-      </c>
-      <c r="G10">
-        <v>0.39818700000000001</v>
+        <v>97</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.55388499999999996</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.43445699999999998</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.399752</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>10</v>
@@ -1461,15 +1535,14 @@
         <v>10</v>
       </c>
       <c r="Q10">
-        <v>0.54530100000000004</v>
+        <v>0.65119400000000005</v>
       </c>
       <c r="R10">
-        <v>0.29455399999999998</v>
+        <v>0.37376199999999998</v>
       </c>
       <c r="S10">
-        <v>0.269202</v>
-      </c>
-      <c r="T10" s="2"/>
+        <v>0.35938599999999998</v>
+      </c>
       <c r="U10" s="8" t="s">
         <v>10</v>
       </c>
@@ -1477,7 +1550,7 @@
         <v>10</v>
       </c>
       <c r="AF10" s="2"/>
-      <c r="AG10" s="23"/>
+      <c r="AG10" s="2"/>
       <c r="AM10" s="8"/>
       <c r="AR10" s="8"/>
     </row>
@@ -1489,7 +1562,7 @@
         <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E11">
         <v>0.55785499999999999</v>
@@ -1516,13 +1589,13 @@
         <v>21</v>
       </c>
       <c r="Q11">
-        <v>0.497809</v>
+        <v>0.60360100000000005</v>
       </c>
       <c r="R11">
-        <v>0.316832</v>
+        <v>0.38613900000000001</v>
       </c>
       <c r="S11">
-        <v>0.297539</v>
+        <v>0.38092100000000001</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="8" t="s">
@@ -1531,7 +1604,7 @@
       <c r="AA11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AG11" s="23"/>
+      <c r="AG11" s="2"/>
       <c r="AM11" s="8"/>
       <c r="AR11" s="8"/>
     </row>
@@ -1543,11 +1616,11 @@
         <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
       <c r="I12" s="9" t="s">
         <v>11</v>
       </c>
@@ -1566,7 +1639,7 @@
       <c r="AA12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AG12" s="24"/>
+      <c r="AG12" s="20"/>
       <c r="AM12" s="9"/>
       <c r="AR12" s="9"/>
     </row>
@@ -1578,7 +1651,7 @@
         <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E13">
         <v>0.55179900000000004</v>
@@ -1605,13 +1678,13 @@
         <v>12</v>
       </c>
       <c r="Q13">
-        <v>0.54598999999999998</v>
+        <v>0.54545100000000002</v>
       </c>
       <c r="R13">
         <v>0.35396</v>
       </c>
       <c r="S13">
-        <v>0.34911799999999998</v>
+        <v>0.34864600000000001</v>
       </c>
       <c r="T13" s="2"/>
       <c r="U13" s="8" t="s">
@@ -1640,7 +1713,7 @@
         <v>0.556975</v>
       </c>
       <c r="AF13" s="2"/>
-      <c r="AG13" s="23"/>
+      <c r="AG13" s="2"/>
       <c r="AM13" s="8"/>
       <c r="AR13" s="8"/>
     </row>
@@ -1652,7 +1725,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14">
         <v>0.49582300000000001</v>
@@ -1679,13 +1752,13 @@
         <v>13</v>
       </c>
       <c r="Q14">
-        <v>0.43309799999999998</v>
+        <v>0.54384200000000005</v>
       </c>
       <c r="R14">
-        <v>0.341584</v>
+        <v>0.36386099999999999</v>
       </c>
       <c r="S14">
-        <v>0.319803</v>
+        <v>0.35640300000000003</v>
       </c>
       <c r="U14" s="8" t="s">
         <v>13</v>
@@ -1693,7 +1766,7 @@
       <c r="AA14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AG14" s="23"/>
+      <c r="AG14" s="2"/>
       <c r="AM14" s="8"/>
       <c r="AR14" s="8"/>
     </row>
@@ -1729,15 +1802,14 @@
         <v>14</v>
       </c>
       <c r="Q15">
-        <v>0.60474300000000003</v>
+        <v>0.60311099999999995</v>
       </c>
       <c r="R15">
         <v>0.41831699999999999</v>
       </c>
       <c r="S15">
-        <v>0.41343099999999999</v>
-      </c>
-      <c r="T15" s="2"/>
+        <v>0.41251700000000002</v>
+      </c>
       <c r="U15" s="8" t="s">
         <v>14</v>
       </c>
@@ -1763,7 +1835,7 @@
       <c r="AE15">
         <v>0.55549099999999996</v>
       </c>
-      <c r="AG15" s="23"/>
+      <c r="AG15" s="2"/>
       <c r="AM15" s="8"/>
       <c r="AR15" s="8"/>
     </row>
@@ -1799,19 +1871,28 @@
         <v>15</v>
       </c>
       <c r="Q16">
-        <v>0.55871099999999996</v>
+        <v>0.55774000000000001</v>
       </c>
       <c r="R16">
         <v>0.485149</v>
       </c>
       <c r="S16">
-        <v>0.47761999999999999</v>
+        <v>0.476937</v>
       </c>
       <c r="T16" s="2"/>
       <c r="U16" s="8" t="s">
         <v>15</v>
       </c>
       <c r="V16" s="15"/>
+      <c r="W16">
+        <v>0.70927600000000002</v>
+      </c>
+      <c r="X16">
+        <v>0.60299599999999998</v>
+      </c>
+      <c r="Y16">
+        <v>0.59994999999999998</v>
+      </c>
       <c r="AA16" s="8" t="s">
         <v>15</v>
       </c>
@@ -1824,14 +1905,14 @@
       <c r="AE16" s="14">
         <v>0.57348399999999999</v>
       </c>
-      <c r="AG16" s="23"/>
+      <c r="AG16" s="2"/>
       <c r="AM16" s="8"/>
       <c r="AR16" s="8"/>
       <c r="AS16" s="2"/>
       <c r="AT16" s="2"/>
       <c r="AU16" s="2"/>
     </row>
-    <row r="17" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
         <v>16</v>
       </c>
@@ -1863,18 +1944,27 @@
         <v>16</v>
       </c>
       <c r="Q17">
-        <v>0.60226999999999997</v>
+        <v>0.60215300000000005</v>
       </c>
       <c r="R17">
         <v>0.235149</v>
       </c>
       <c r="S17">
-        <v>0.191112</v>
+        <v>0.190939</v>
       </c>
       <c r="U17" s="8" t="s">
         <v>16</v>
       </c>
       <c r="V17" s="16"/>
+      <c r="W17">
+        <v>0.57190099999999999</v>
+      </c>
+      <c r="X17">
+        <v>0.45880100000000001</v>
+      </c>
+      <c r="Y17">
+        <v>0.401509</v>
+      </c>
       <c r="AA17" s="8" t="s">
         <v>16</v>
       </c>
@@ -1887,11 +1977,11 @@
       <c r="AE17">
         <v>0.34958600000000001</v>
       </c>
-      <c r="AG17" s="23"/>
+      <c r="AG17" s="2"/>
       <c r="AM17" s="8"/>
       <c r="AR17" s="8"/>
     </row>
-    <row r="18" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B18" s="9" t="s">
         <v>17</v>
       </c>
@@ -1899,11 +1989,11 @@
         <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
       <c r="I18" s="9" t="s">
         <v>17</v>
       </c>
@@ -1922,11 +2012,11 @@
       <c r="AA18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AG18" s="24"/>
+      <c r="AG18" s="20"/>
       <c r="AM18" s="9"/>
       <c r="AR18" s="9"/>
     </row>
-    <row r="19" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
         <v>18</v>
       </c>
@@ -1934,7 +2024,7 @@
         <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19">
         <v>0.53071400000000002</v>
@@ -1961,13 +2051,13 @@
         <v>18</v>
       </c>
       <c r="Q19">
-        <v>0.43840600000000002</v>
+        <v>0.55005899999999996</v>
       </c>
       <c r="R19">
-        <v>0.27722799999999997</v>
+        <v>0.329208</v>
       </c>
       <c r="S19">
-        <v>0.237849</v>
+        <v>0.30829699999999999</v>
       </c>
       <c r="U19" s="8" t="s">
         <v>18</v>
@@ -1975,11 +2065,11 @@
       <c r="AA19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="AG19" s="23"/>
+      <c r="AG19" s="2"/>
       <c r="AM19" s="8"/>
       <c r="AR19" s="8"/>
     </row>
-    <row r="20" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
         <v>93</v>
       </c>
@@ -1987,7 +2077,7 @@
         <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E20">
         <v>0.51036099999999995</v>
@@ -2014,13 +2104,13 @@
         <v>93</v>
       </c>
       <c r="Q20">
-        <v>0.52865600000000001</v>
+        <v>0.56456899999999999</v>
       </c>
       <c r="R20">
-        <v>0.28960399999999997</v>
+        <v>0.344059</v>
       </c>
       <c r="S20">
-        <v>0.26192700000000002</v>
+        <v>0.325963</v>
       </c>
       <c r="U20" s="8" t="s">
         <v>93</v>
@@ -2028,11 +2118,11 @@
       <c r="AA20" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="AG20" s="23"/>
+      <c r="AG20" s="2"/>
       <c r="AM20" s="8"/>
       <c r="AR20" s="8"/>
     </row>
-    <row r="21" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
@@ -2064,13 +2154,13 @@
         <v>24</v>
       </c>
       <c r="Q21">
-        <v>0.47489900000000002</v>
+        <v>0.47480299999999998</v>
       </c>
       <c r="R21">
         <v>0.28712900000000002</v>
       </c>
       <c r="S21">
-        <v>0.25231799999999999</v>
+        <v>0.25218800000000002</v>
       </c>
       <c r="U21" s="8" t="s">
         <v>24</v>
@@ -2078,16 +2168,16 @@
       <c r="AA21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AG21" s="23"/>
+      <c r="AG21" s="2"/>
       <c r="AM21" s="8"/>
       <c r="AR21" s="8"/>
     </row>
-    <row r="22" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B22" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E22">
         <v>0.57200399999999996</v>
@@ -2114,13 +2204,13 @@
         <v>25</v>
       </c>
       <c r="Q22">
-        <v>0.499913</v>
+        <v>0.61236900000000005</v>
       </c>
       <c r="R22">
-        <v>0.329208</v>
+        <v>0.38861400000000001</v>
       </c>
       <c r="S22">
-        <v>0.30395699999999998</v>
+        <v>0.38125700000000001</v>
       </c>
       <c r="U22" s="8" t="s">
         <v>25</v>
@@ -2128,19 +2218,19 @@
       <c r="AA22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AG22" s="23"/>
+      <c r="AG22" s="2"/>
       <c r="AM22" s="8"/>
       <c r="AR22" s="8"/>
     </row>
-    <row r="23" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B23" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E23">
         <v>0.57674099999999995</v>
@@ -2167,13 +2257,13 @@
         <v>26</v>
       </c>
       <c r="Q23">
-        <v>0.46459899999999998</v>
+        <v>0.56205499999999997</v>
       </c>
       <c r="R23">
-        <v>0.30940600000000001</v>
+        <v>0.37623800000000002</v>
       </c>
       <c r="S23">
-        <v>0.28628999999999999</v>
+        <v>0.36523600000000001</v>
       </c>
       <c r="U23" s="8" t="s">
         <v>26</v>
@@ -2181,19 +2271,19 @@
       <c r="AA23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AG23" s="23"/>
+      <c r="AG23" s="2"/>
       <c r="AM23" s="8"/>
       <c r="AR23" s="8"/>
     </row>
-    <row r="24" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E24">
         <v>0.57912399999999997</v>
@@ -2220,13 +2310,13 @@
         <v>27</v>
       </c>
       <c r="Q24">
-        <v>0.48017300000000002</v>
+        <v>0.58631999999999995</v>
       </c>
       <c r="R24">
-        <v>0.30198000000000003</v>
+        <v>0.36633700000000002</v>
       </c>
       <c r="S24">
-        <v>0.27839900000000001</v>
+        <v>0.35813699999999998</v>
       </c>
       <c r="U24" s="8" t="s">
         <v>27</v>
@@ -2234,11 +2324,11 @@
       <c r="AA24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AG24" s="23"/>
+      <c r="AG24" s="2"/>
       <c r="AM24" s="8"/>
       <c r="AR24" s="8"/>
     </row>
-    <row r="25" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
@@ -2246,7 +2336,7 @@
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E25">
         <v>0.63638499999999998</v>
@@ -2273,19 +2363,27 @@
         <v>28</v>
       </c>
       <c r="Q25">
-        <v>0.60309599999999997</v>
+        <v>0.601464</v>
       </c>
       <c r="R25">
         <v>0.41831699999999999</v>
       </c>
       <c r="S25">
-        <v>0.41634399999999999</v>
-      </c>
-      <c r="T25" s="2"/>
+        <v>0.41543000000000002</v>
+      </c>
       <c r="U25" s="8" t="s">
         <v>28</v>
       </c>
       <c r="V25" s="16"/>
+      <c r="W25">
+        <v>0.68159099999999995</v>
+      </c>
+      <c r="X25">
+        <v>0.58801499999999995</v>
+      </c>
+      <c r="Y25">
+        <v>0.58170900000000003</v>
+      </c>
       <c r="Z25" s="5"/>
       <c r="AA25" s="8" t="s">
         <v>28</v>
@@ -2299,19 +2397,19 @@
       <c r="AE25">
         <v>0.560608</v>
       </c>
-      <c r="AG25" s="23"/>
+      <c r="AG25" s="2"/>
       <c r="AM25" s="8"/>
       <c r="AR25" s="8"/>
     </row>
-    <row r="26" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E26">
         <v>0.60144699999999995</v>
@@ -2338,19 +2436,28 @@
         <v>29</v>
       </c>
       <c r="Q26">
-        <v>0.53626799999999997</v>
+        <v>0.53548600000000002</v>
       </c>
       <c r="R26">
         <v>0.43069299999999999</v>
       </c>
       <c r="S26">
-        <v>0.42550700000000002</v>
+        <v>0.42490800000000001</v>
       </c>
       <c r="T26" s="2"/>
       <c r="U26" s="8" t="s">
         <v>29</v>
       </c>
       <c r="V26" s="16"/>
+      <c r="W26">
+        <v>0.70315899999999998</v>
+      </c>
+      <c r="X26">
+        <v>0.60112399999999999</v>
+      </c>
+      <c r="Y26">
+        <v>0.59575299999999998</v>
+      </c>
       <c r="AA26" s="8" t="s">
         <v>29</v>
       </c>
@@ -2363,19 +2470,19 @@
       <c r="AE26">
         <v>0.57139099999999998</v>
       </c>
-      <c r="AG26" s="23"/>
+      <c r="AG26" s="2"/>
       <c r="AM26" s="8"/>
       <c r="AR26" s="8"/>
     </row>
-    <row r="27" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B27" s="8" t="s">
         <v>91</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E27">
         <v>0.55141600000000002</v>
@@ -2402,13 +2509,13 @@
         <v>91</v>
       </c>
       <c r="Q27">
-        <v>0.61195900000000003</v>
+        <v>0.59537499999999999</v>
       </c>
       <c r="R27">
-        <v>0.35643599999999998</v>
+        <v>0.36386099999999999</v>
       </c>
       <c r="S27">
-        <v>0.34517799999999998</v>
+        <v>0.356153</v>
       </c>
       <c r="U27" s="8" t="s">
         <v>91</v>
@@ -2416,11 +2523,11 @@
       <c r="AA27" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="AG27" s="23"/>
+      <c r="AG27" s="2"/>
       <c r="AM27" s="8"/>
       <c r="AR27" s="8"/>
     </row>
-    <row r="28" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
         <v>92</v>
       </c>
@@ -2452,13 +2559,13 @@
         <v>92</v>
       </c>
       <c r="Q28">
-        <v>0.55375399999999997</v>
+        <v>0.528613</v>
       </c>
       <c r="R28">
-        <v>0.27722799999999997</v>
+        <v>0.31188100000000002</v>
       </c>
       <c r="S28">
-        <v>0.24971199999999999</v>
+        <v>0.29010399999999997</v>
       </c>
       <c r="U28" s="8" t="s">
         <v>92</v>
@@ -2466,38 +2573,147 @@
       <c r="AA28" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="AG28" s="23"/>
+      <c r="AG28" s="2"/>
       <c r="AM28" s="8"/>
       <c r="AR28" s="8"/>
     </row>
-    <row r="29" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="AG29" s="23"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A29" s="26"/>
+      <c r="B29" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29">
+        <v>0.57575100000000001</v>
+      </c>
+      <c r="F29">
+        <v>0.45880100000000001</v>
+      </c>
+      <c r="G29">
+        <v>0.421572</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="K29">
+        <v>0.59193499999999999</v>
+      </c>
+      <c r="L29">
+        <v>0.45880100000000001</v>
+      </c>
+      <c r="M29">
+        <v>0.42186299999999999</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="U29" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG29" s="2"/>
+    </row>
+    <row r="30" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A30" s="26"/>
+      <c r="B30" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30">
+        <v>0.604819</v>
+      </c>
+      <c r="F30">
+        <v>0.46441900000000003</v>
+      </c>
+      <c r="G30">
+        <v>0.44495600000000002</v>
+      </c>
+      <c r="I30" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="K30">
+        <v>0.60010799999999997</v>
+      </c>
+      <c r="L30">
+        <v>0.45318399999999998</v>
+      </c>
+      <c r="M30">
+        <v>0.43686399999999997</v>
+      </c>
+      <c r="O30" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="U30" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="V30" s="16"/>
+      <c r="W30">
+        <v>0.66785799999999995</v>
+      </c>
+      <c r="X30">
+        <v>0.56928800000000002</v>
+      </c>
+      <c r="Y30">
+        <v>0.56293199999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:25" x14ac:dyDescent="0.2">
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:25" x14ac:dyDescent="0.2">
       <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="W34" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="X34" s="27"/>
+      <c r="Y34" s="27"/>
+    </row>
+    <row r="35" spans="2:25" x14ac:dyDescent="0.2">
       <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y35" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="K36" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U36" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="W36">
+        <v>0.469831</v>
+      </c>
+      <c r="X36">
+        <v>0.25742599999999999</v>
+      </c>
+      <c r="Y36">
+        <v>0.210198</v>
+      </c>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>1</v>
       </c>
@@ -2522,8 +2738,20 @@
       <c r="M37" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U37" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="W37">
+        <v>0.65417800000000004</v>
+      </c>
+      <c r="X37">
+        <v>0.225248</v>
+      </c>
+      <c r="Y37">
+        <v>0.17084299999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B38" s="8" t="s">
         <v>5</v>
       </c>
@@ -2546,153 +2774,412 @@
       <c r="M38">
         <v>0.904613</v>
       </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U38" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="W38" s="12"/>
+      <c r="X38" s="12"/>
+      <c r="Y38" s="12"/>
+    </row>
+    <row r="39" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B39" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="11"/>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U39" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="W39" s="12"/>
+      <c r="X39" s="12"/>
+      <c r="Y39" s="12"/>
+    </row>
+    <row r="40" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B40" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C40" s="11"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U40" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="W40">
+        <v>0.59226599999999996</v>
+      </c>
+      <c r="X40">
+        <v>0.31930700000000001</v>
+      </c>
+      <c r="Y40">
+        <v>0.29668600000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B41" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C41" s="11"/>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U41" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="W41">
+        <v>0.48905399999999999</v>
+      </c>
+      <c r="X41">
+        <v>0.31188100000000002</v>
+      </c>
+      <c r="Y41">
+        <v>0.29295399999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B42" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C42" s="11"/>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U42" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="W42">
+        <v>0.54530100000000004</v>
+      </c>
+      <c r="X42">
+        <v>0.29455399999999998</v>
+      </c>
+      <c r="Y42">
+        <v>0.269202</v>
+      </c>
+    </row>
+    <row r="43" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B43" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="11"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U43" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="W43">
+        <v>0.497809</v>
+      </c>
+      <c r="X43">
+        <v>0.316832</v>
+      </c>
+      <c r="Y43">
+        <v>0.297539</v>
+      </c>
+    </row>
+    <row r="44" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B44" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C44" s="11"/>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W44" s="12"/>
+      <c r="X44" s="12"/>
+      <c r="Y44" s="12"/>
+    </row>
+    <row r="45" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B45" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C45" s="11"/>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U45" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="W45">
+        <v>0.54598999999999998</v>
+      </c>
+      <c r="X45">
+        <v>0.35396</v>
+      </c>
+      <c r="Y45">
+        <v>0.34911799999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B46" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C46" s="11"/>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U46" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="W46">
+        <v>0.43309799999999998</v>
+      </c>
+      <c r="X46">
+        <v>0.341584</v>
+      </c>
+      <c r="Y46">
+        <v>0.319803</v>
+      </c>
+    </row>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B47" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C47" s="11"/>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="U47" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="W47">
+        <v>0.60474300000000003</v>
+      </c>
+      <c r="X47">
+        <v>0.41831699999999999</v>
+      </c>
+      <c r="Y47">
+        <v>0.41343099999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B48" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C48" s="11"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U48" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="W48">
+        <v>0.55871099999999996</v>
+      </c>
+      <c r="X48">
+        <v>0.485149</v>
+      </c>
+      <c r="Y48">
+        <v>0.47761999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B49" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C49" s="11"/>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U49" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="W49">
+        <v>0.60226999999999997</v>
+      </c>
+      <c r="X49">
+        <v>0.235149</v>
+      </c>
+      <c r="Y49">
+        <v>0.191112</v>
+      </c>
+    </row>
+    <row r="50" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B50" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C50" s="11"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U50" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="W50" s="12"/>
+      <c r="X50" s="12"/>
+      <c r="Y50" s="12"/>
+    </row>
+    <row r="51" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B51" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C51" s="11"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U51" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="W51">
+        <v>0.43840600000000002</v>
+      </c>
+      <c r="X51">
+        <v>0.27722799999999997</v>
+      </c>
+      <c r="Y51">
+        <v>0.237849</v>
+      </c>
+    </row>
+    <row r="52" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B52" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C52" s="11"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U52" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="W52">
+        <v>0.52865600000000001</v>
+      </c>
+      <c r="X52">
+        <v>0.28960399999999997</v>
+      </c>
+      <c r="Y52">
+        <v>0.26192700000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B53" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C53" s="11"/>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U53" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="W53">
+        <v>0.47489900000000002</v>
+      </c>
+      <c r="X53">
+        <v>0.28712900000000002</v>
+      </c>
+      <c r="Y53">
+        <v>0.25231799999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B54" s="8" t="s">
         <v>93</v>
       </c>
       <c r="C54" s="11"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U54" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="W54">
+        <v>0.499913</v>
+      </c>
+      <c r="X54">
+        <v>0.329208</v>
+      </c>
+      <c r="Y54">
+        <v>0.30395699999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B55" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C55" s="11"/>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U55" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="W55">
+        <v>0.46459899999999998</v>
+      </c>
+      <c r="X55">
+        <v>0.30940600000000001</v>
+      </c>
+      <c r="Y55">
+        <v>0.28628999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B56" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C56" s="11"/>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U56" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="W56">
+        <v>0.48017300000000002</v>
+      </c>
+      <c r="X56">
+        <v>0.30198000000000003</v>
+      </c>
+      <c r="Y56">
+        <v>0.27839900000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B57" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C57" s="11"/>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U57" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="W57">
+        <v>0.60309599999999997</v>
+      </c>
+      <c r="X57">
+        <v>0.41831699999999999</v>
+      </c>
+      <c r="Y57">
+        <v>0.41634399999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B58" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C58" s="11"/>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U58" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="W58">
+        <v>0.53626799999999997</v>
+      </c>
+      <c r="X58">
+        <v>0.43069299999999999</v>
+      </c>
+      <c r="Y58">
+        <v>0.42550700000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B59" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C59" s="11"/>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U59" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="W59">
+        <v>0.61195900000000003</v>
+      </c>
+      <c r="X59">
+        <v>0.35643599999999998</v>
+      </c>
+      <c r="Y59">
+        <v>0.34517799999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B60" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C60" s="11"/>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U60" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="W60">
+        <v>0.55375399999999997</v>
+      </c>
+      <c r="X60">
+        <v>0.27722799999999997</v>
+      </c>
+      <c r="Y60">
+        <v>0.24971199999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B61" s="8" t="s">
         <v>91</v>
       </c>
       <c r="C61" s="11"/>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="U61" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B62" s="8" t="s">
         <v>92</v>
       </c>
       <c r="C62" s="11"/>
+      <c r="U62" s="25" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="W34:Y34"/>
     <mergeCell ref="AN2:AP2"/>
     <mergeCell ref="AS2:AU2"/>
     <mergeCell ref="Q2:S2"/>
@@ -4621,8 +5108,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4696,20 +5183,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="G1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -5312,20 +5799,20 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="G43" s="22" t="s">
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="G43" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">

</xml_diff>